<commit_message>
Rule Loading Exception added
</commit_message>
<xml_diff>
--- a/src/main/Configuration/Rules_V2.xlsx
+++ b/src/main/Configuration/Rules_V2.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M2_Sorbonne\Projet_Moteur\Rule_Engine\src\main\Configuration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,195 +24,195 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="134">
-  <si>
-    <t xml:space="preserve">Workflow name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TYPE_TITRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TYPE_TITRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TYPE_DEMANDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TYPE_DEMANDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DATE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DATE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_STATUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_STATUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_SEXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_SEXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM_USUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM_USUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TAILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TAILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_VILLE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_VILLE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PAYS_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PAYS_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DEPARTEMENT_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DEPARTEMENT_NAISSSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_YEUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_YEUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_ORIGINE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_ORIGINE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_REPRESENTANT_LEGAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_REPRESANTANT_LEGAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_ADRESSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_ADRESSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_CODE_POSTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_CODE_POSTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_COMMUNE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_COMMUNE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TEL_PORTABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TEL_PORTABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DATE_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DATE_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_LIEU_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_LIEU_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NATIONALITE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NATIONALITE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DATE_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DATE_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_LIEU_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_LIEU_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NATIONALITE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NATIONALITE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande passeport mineur</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="135">
+  <si>
+    <t>Workflow name</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>REGLE_TYPE_TITRE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TYPE_TITRE</t>
+  </si>
+  <si>
+    <t>REGLE_TYPE_DEMANDE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TYPE_DEMANDE</t>
+  </si>
+  <si>
+    <t>REGLE_DATE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DATE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM</t>
+  </si>
+  <si>
+    <t>REGLE_NOM</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM</t>
+  </si>
+  <si>
+    <t>REGLE_STATUT</t>
+  </si>
+  <si>
+    <t>MESSAGE_STATUT</t>
+  </si>
+  <si>
+    <t>REGLE_SEXE</t>
+  </si>
+  <si>
+    <t>MESSAGE_SEXE</t>
+  </si>
+  <si>
+    <t>REGLE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM_USUEL</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM_USUEL</t>
+  </si>
+  <si>
+    <t>REGLE_TAILLE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TAILLE</t>
+  </si>
+  <si>
+    <t>REGLE_VILLE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_VILLE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_PAYS_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_PAYS_NAISSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_DEPARTEMENT_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DEPARTEMENT_NAISSSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_YEUX</t>
+  </si>
+  <si>
+    <t>MESSAGE_YEUX</t>
+  </si>
+  <si>
+    <t>REGLE_ORIGINE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>MESSAGE_ORIGINE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>REGLE_REPRESENTANT_LEGAL</t>
+  </si>
+  <si>
+    <t>MESSAGE_REPRESANTANT_LEGAL</t>
+  </si>
+  <si>
+    <t>REGLE_ADRESSE</t>
+  </si>
+  <si>
+    <t>MESSAGE_ADRESSE</t>
+  </si>
+  <si>
+    <t>REGLE_CODE_POSTAL</t>
+  </si>
+  <si>
+    <t>MESSAGE_CODE_POSTAL</t>
+  </si>
+  <si>
+    <t>REGLE_COMMUNE</t>
+  </si>
+  <si>
+    <t>MESSAGE_COMMUNE</t>
+  </si>
+  <si>
+    <t>REGLE_TEL_PORTABLE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TEL_PORTABLE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_NOM_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_DATE_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DATE_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_LIEU_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_LIEU_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_NATIONALITE_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NATIONALITE_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_NOM_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_DATE_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DATE_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_LIEU_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_LIEU_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_NATIONALITE_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NATIONALITE_MERE</t>
+  </si>
+  <si>
+    <t>Première Demande passeport mineur</t>
   </si>
   <si>
     <r>
@@ -228,11 +232,11 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">"PREMIERE DEMANDE")</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; Equal(value,"PSP")</t>
+      <t>"PREMIERE DEMANDE")</t>
+    </r>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; Equal(value,"PSP")</t>
   </si>
   <si>
     <r>
@@ -252,7 +256,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">"PSP".</t>
+      <t>"PSP".</t>
     </r>
   </si>
   <si>
@@ -273,23 +277,23 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">"PREMIERE DEMANDE")</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Il doit contenir "PREMIERE DEMANDE".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp;  Minor_Check(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Doit être un mineur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; Length_Between(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
+      <t>"PREMIERE DEMANDE")</t>
+    </r>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Il doit contenir "PREMIERE DEMANDE".</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp;  Minor_Check(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Doit être un mineur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; Length_Between(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
   </si>
   <si>
     <r>
@@ -310,7 +314,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">"</t>
+      <t>"</t>
     </r>
     <r>
       <rPr>
@@ -320,7 +324,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">mineur,MINEUR,Mineur</t>
+      <t>mineur,MINEUR,Mineur</t>
     </r>
     <r>
       <rPr>
@@ -330,7 +334,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">"</t>
+      <t>"</t>
     </r>
     <r>
       <rPr>
@@ -340,48 +344,48 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et correspond l’un des mots suivant : mineur,MINEUR,Mineur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; BelongTo(value,"F,H,femme,homme,Femme,Homme,FEMME,HOMME")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et correspond l’un des mots suivant : F,H,femme,homme,Femme,Homme,FEMME,HOMME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(NotNull(value) &amp;&amp; Length_Between(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")) || IsNull(value)</t>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et correspond l’un des mots suivant : mineur,MINEUR,Mineur</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; BelongTo(value,"F,H,femme,homme,Femme,Homme,FEMME,HOMME")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et correspond l’un des mots suivant : F,H,femme,homme,Femme,Homme,FEMME,HOMME</t>
+  </si>
+  <si>
+    <t>(NotNull(value) &amp;&amp; Length_Between(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")) || IsNull(value)</t>
   </si>
   <si>
     <t xml:space="preserve"> La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; IsFloat(TAILLE)
+    <t>NotNull(value) &amp;&amp; IsFloat(TAILLE)
 &amp;&amp; Float_Between(value,0.5,3.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ce champ est obligatoire. La taille doit être dans un intervalle de 0,5 et 3,0m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( BornInFrance(PAYS_NAISSANCE) &amp;&amp; NotNull(value)   &amp;&amp; Length_Less_Than(value,3) &amp;&amp; IsNumber(value)) ||( !BornInFrance(PAYS_NAISSANCE) &amp;&amp; IsNull(value) )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si le champ PAYS_NAISSANCE est égale à France alors ce champ est obligatoire. La taille ne doit pas dépasser 3.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est toujours valide pour ce workflow</t>
+    <t>Ce champ est obligatoire. La taille doit être dans un intervalle de 0,5 et 3,0m</t>
+  </si>
+  <si>
+    <t>NotNull(value)</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire.</t>
+  </si>
+  <si>
+    <t>( BornInFrance(PAYS_NAISSANCE) &amp;&amp; NotNull(value)   &amp;&amp; Length_Less_Than(value,3) &amp;&amp; IsNumber(value)) ||( !BornInFrance(PAYS_NAISSANCE) &amp;&amp; IsNull(value) )</t>
+  </si>
+  <si>
+    <t>Si le champ PAYS_NAISSANCE est égale à France alors ce champ est obligatoire. La taille ne doit pas dépasser 3.</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>Ce champ est toujours valide pour ce workflow</t>
   </si>
   <si>
     <r>
@@ -402,41 +406,41 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Si le champ NOM_USAGE n’est pas vide alors ce champ est obligatoire et doit correspondre l’une des valeur suivants : Père,Mère,Époux,Épouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les carectère : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; IsNumber(value)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; IsNumber(value) &amp;&amp; LengthEqual(value,10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et doit être un nombre de 10 chiffres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
+      <t>NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
+    </r>
+  </si>
+  <si>
+    <t>Si le champ NOM_USAGE n’est pas vide alors ce champ est obligatoire et doit correspondre l’une des valeur suivants : Père,Mère,Époux,Épouse</t>
+  </si>
+  <si>
+    <t>Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les carectère : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; IsNumber(value)</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; IsNumber(value) &amp;&amp; LengthEqual(value,10)</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et doit être un nombre de 10 chiffres</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
   </si>
   <si>
     <t xml:space="preserve">NotNull(value) </t>
   </si>
   <si>
-    <t xml:space="preserve">Première Demande CNIE mineur</t>
+    <t>Première Demande CNIE mineur</t>
   </si>
   <si>
     <r>
@@ -445,10 +449,21 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">NotNull(value) &amp;&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
-    </r>
+      <t>Equal(value,"CNIE")</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -456,16 +471,47 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
-    </r>
-  </si>
-  <si>
+      <t xml:space="preserve">Ce champ est obligatoire. </t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">C’est une demande de pièce d’identité. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Il doit contenir "CNIE".</t>
+    </r>
+  </si>
+  <si>
+    <t>NotNull(value)&amp;&amp; BelongTo(value, "mineur,MINEUR,Mineur")</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; BelongTo(value,"marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT")</t>
+  </si>
+  <si>
+    <t>Le champ est obligatoire et doit correspondre à l’un des valeur suivants : marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT</t>
+  </si>
+  <si>
+    <t>Première Demande passeport adulte</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">NotNull(value) &amp;&amp; </t>
     </r>
@@ -477,7 +523,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Equal(value,"CNIE")</t>
+      <t>Equal(value,"PSP")</t>
     </r>
   </si>
   <si>
@@ -498,7 +544,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">C’est une demande de pièce d’identité. </t>
+      <t xml:space="preserve">C’est une demande de passeport. </t>
     </r>
     <r>
       <rPr>
@@ -507,20 +553,23 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Il doit contenir "CNIE".</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)&amp;&amp; BelongTo(value, "mineur,MINEUR,Mineur")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; BelongTo(value,"marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire et doit correspondre à l’un des valeur suivants : marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande passeport adulte</t>
+      <t>Il doit contenir "PSP".</t>
+    </r>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; Major_Check(value)  &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Doit être un majeur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>NotNull(value)&amp;&amp; BelongTo(value,"majeur,MAJEUR,Majeur")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et correspond l’un des mots suivant : majeur,MAJEUR,Majeur</t>
+  </si>
+  <si>
+    <t>Première Demande CNIE adulte</t>
   </si>
   <si>
     <r>
@@ -531,19 +580,276 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" )  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
+    </r>
+  </si>
+  <si>
+    <t>Première Demande passeport mineur emancipé</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
+    </r>
+  </si>
+  <si>
+    <t>NotNull(value)   &amp;&amp;  Minor_Check(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Première Demande CNIE mineur emancipé</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BelongTo(STATUT, "mineur,MINEUR,Mineur") </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
+    </r>
+  </si>
+  <si>
+    <t>Renouvellement passeport mineur</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"RENOUVELLEMENT")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">NotNull(value) &amp;&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Equal(value,"PSP")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ce champ est obligatoire. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>C’est une demande de passeport.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Il doit contenir "PSP".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NotNull(value) &amp;&amp; Equal(value, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"RENOUVELLEMENT")</t>
+    </r>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Il doit contenir "RENOUVELLEMENT".</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le champ est obligatoire et la longueur doit être entre 1 et 76 </t>
+  </si>
+  <si>
+    <t>Renouvellement CNIE mineur</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BelongTo(STATUT, "mineur,MINEUR,Mineur") </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"RENOUVELLEMENT")</t>
+    </r>
+  </si>
+  <si>
+    <t>Renouvellement passeport adulte</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" ) &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"RENOUVELLEMENT")</t>
+    </r>
+  </si>
+  <si>
+    <t>Renouvellement CNIE adulte</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
-    </r>
-  </si>
-  <si>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ce  champ est obligatoire. C’est une demande de pièce d’identité. </t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -551,383 +857,27 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">NotNull(value) &amp;&amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Equal(value,"PSP")</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ce champ est obligatoire. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C’est une demande de passeport. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Il doit contenir "PSP".</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; Major_Check(value)  &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Doit être un majeur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)&amp;&amp; BelongTo(value,"majeur,MAJEUR,Majeur")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et correspond l’un des mots suivant : majeur,MAJEUR,Majeur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande CNIE adulte</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" )  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande passeport mineur emancipé</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)   &amp;&amp;  Minor_Check(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande CNIE mineur emancipé</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BelongTo(STATUT, "mineur,MINEUR,Mineur") </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Renouvellement passeport mineur</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"RENOUVELLEMENT")</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">NotNull(value) &amp;&amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Equal(value,"PSP")</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ce champ est obligatoire. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C’est une demande de passeport.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Il doit contenir "PSP".</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NotNull(value) &amp;&amp; Equal(value, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"RENOUVELLEMENT")</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Il doit contenir "RENOUVELLEMENT".</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire et la longueur doit être entre 1 et 76 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renouvellement CNIE mineur</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BelongTo(STATUT, "mineur,MINEUR,Mineur") </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"RENOUVELLEMENT")</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Renouvellement passeport adulte</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" ) &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"RENOUVELLEMENT")</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Renouvellement CNIE adulte</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">  NotNull(DATE_NAISSANCE) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" )  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"RENOUVELLEMENT")</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Ce  champ est obligatoire. C’est une demande de pièce d’identité. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Il doit contenir "CNIE".</t>
-    </r>
+      <t>Il doit contenir "CNIE".</t>
+    </r>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; Equal(value,"CNIE")</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "CNIE") &amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" ) &amp;&amp;  Equal(TYPE_TITRE, "PSP") &amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"PREMIERE DEMANDE")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  NotNull(DATE_NAISSANCE) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" )  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") &amp;&amp; NotNull(TYPE_DEMANDE) &amp;&amp; Equal(TYPE_DEMANDE,"RENOUVELLEMENT")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -936,22 +886,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -1006,15 +941,17 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="thin">
         <color rgb="FF5B9BD5"/>
@@ -1024,7 +961,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1035,120 +972,84 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF5B9BD5"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF5B9BD5"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1207,60 +1108,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1292,7 +1209,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -1316,7 +1233,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1376,68 +1293,66 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BD2" activeCellId="0" sqref="BD2:BD11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="64.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="27.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="61.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="66.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="48.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="62.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="23" style="2" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="90"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="90"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="2" width="40.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="2" width="74.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="35" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="43" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="47" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="53" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="57" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16353" min="65" style="2" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16356" min="16354" style="2" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16357" min="16357" style="0" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16358" style="0" width="10.16"/>
+    <col min="1" max="1" width="47.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="2" customWidth="1"/>
+    <col min="5" max="7" width="27.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="61.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="54" style="2" customWidth="1"/>
+    <col min="11" max="11" width="66.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="54" style="2" customWidth="1"/>
+    <col min="13" max="13" width="63" style="2" customWidth="1"/>
+    <col min="14" max="14" width="31.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="72" style="2" customWidth="1"/>
+    <col min="16" max="16" width="31.44140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="48.33203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="54" style="2" customWidth="1"/>
+    <col min="19" max="19" width="62.21875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="54" style="2" customWidth="1"/>
+    <col min="21" max="22" width="31.44140625" style="2" customWidth="1"/>
+    <col min="23" max="25" width="22.44140625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="31.44140625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="90" style="2" customWidth="1"/>
+    <col min="28" max="28" width="31.44140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="81" style="2" customWidth="1"/>
+    <col min="30" max="30" width="31.44140625" style="2" customWidth="1"/>
+    <col min="31" max="31" width="90" style="2" customWidth="1"/>
+    <col min="32" max="32" width="40.44140625" style="2" customWidth="1"/>
+    <col min="33" max="33" width="74.44140625" style="2" customWidth="1"/>
+    <col min="34" max="34" width="54" style="2" customWidth="1"/>
+    <col min="35" max="42" width="31.44140625" style="2" customWidth="1"/>
+    <col min="43" max="46" width="54" style="2" customWidth="1"/>
+    <col min="47" max="52" width="31.44140625" style="2" customWidth="1"/>
+    <col min="53" max="56" width="54" style="2" customWidth="1"/>
+    <col min="57" max="64" width="31.44140625" style="2" customWidth="1"/>
+    <col min="65" max="16353" width="8.5546875" style="2"/>
+    <col min="16354" max="16356" width="10.109375" style="2" customWidth="1"/>
+    <col min="16357" max="16384" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:62 16357:16384" s="5" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1624,36 +1539,36 @@
       <c r="BJ1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="XEC1" s="0"/>
-      <c r="XED1" s="0"/>
-      <c r="XEE1" s="0"/>
-      <c r="XEF1" s="0"/>
-      <c r="XEG1" s="0"/>
-      <c r="XEH1" s="0"/>
-      <c r="XEI1" s="0"/>
-      <c r="XEJ1" s="0"/>
-      <c r="XEK1" s="0"/>
-      <c r="XEL1" s="0"/>
-      <c r="XEM1" s="0"/>
-      <c r="XEN1" s="0"/>
-      <c r="XEO1" s="0"/>
-      <c r="XEP1" s="0"/>
-      <c r="XEQ1" s="0"/>
-      <c r="XER1" s="0"/>
-      <c r="XES1" s="0"/>
-      <c r="XET1" s="0"/>
-      <c r="XEU1" s="0"/>
-      <c r="XEV1" s="0"/>
-      <c r="XEW1" s="0"/>
-      <c r="XEX1" s="0"/>
-      <c r="XEY1" s="0"/>
-      <c r="XEZ1" s="0"/>
-      <c r="XFA1" s="0"/>
-      <c r="XFB1" s="0"/>
-      <c r="XFC1" s="0"/>
-      <c r="XFD1" s="0"/>
+      <c r="XEC1"/>
+      <c r="XED1"/>
+      <c r="XEE1"/>
+      <c r="XEF1"/>
+      <c r="XEG1"/>
+      <c r="XEH1"/>
+      <c r="XEI1"/>
+      <c r="XEJ1"/>
+      <c r="XEK1"/>
+      <c r="XEL1"/>
+      <c r="XEM1"/>
+      <c r="XEN1"/>
+      <c r="XEO1"/>
+      <c r="XEP1"/>
+      <c r="XEQ1"/>
+      <c r="XER1"/>
+      <c r="XES1"/>
+      <c r="XET1"/>
+      <c r="XEU1"/>
+      <c r="XEV1"/>
+      <c r="XEW1"/>
+      <c r="XEX1"/>
+      <c r="XEY1"/>
+      <c r="XEZ1"/>
+      <c r="XFA1"/>
+      <c r="XFB1"/>
+      <c r="XFC1"/>
+      <c r="XFD1"/>
     </row>
-    <row r="2" customFormat="false" ht="77.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:62 16357:16384" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
@@ -1841,18 +1756,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:62 16357:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>66</v>
@@ -1879,7 +1794,7 @@
         <v>71</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>73</v>
@@ -1927,10 +1842,10 @@
         <v>83</v>
       </c>
       <c r="AC3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD3" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="AD3" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="AE3" s="12" t="s">
         <v>86</v>
@@ -2029,18 +1944,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:62 16357:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>66</v>
@@ -2049,28 +1964,28 @@
         <v>67</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="N4" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>74</v>
@@ -2217,18 +2132,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:62 16357:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>66</v>
@@ -2237,28 +2152,28 @@
         <v>67</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="N5" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="O5" s="10" t="s">
         <v>74</v>
@@ -2303,10 +2218,10 @@
         <v>83</v>
       </c>
       <c r="AC5" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD5" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="AD5" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="AE5" s="12" t="s">
         <v>86</v>
@@ -2405,18 +2320,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:62 16357:16384" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>66</v>
@@ -2425,10 +2340,10 @@
         <v>67</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>70</v>
@@ -2443,7 +2358,7 @@
         <v>71</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>73</v>
@@ -2491,10 +2406,10 @@
         <v>83</v>
       </c>
       <c r="AC6" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD6" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="AD6" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="AE6" s="12" t="s">
         <v>86</v>
@@ -2593,18 +2508,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:62 16357:16384" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>66</v>
@@ -2613,10 +2528,10 @@
         <v>67</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>70</v>
@@ -2631,7 +2546,7 @@
         <v>71</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N7" s="9" t="s">
         <v>73</v>
@@ -2679,10 +2594,10 @@
         <v>83</v>
       </c>
       <c r="AC7" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD7" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="AD7" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="AE7" s="12" t="s">
         <v>86</v>
@@ -2781,24 +2696,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:62 16357:16384" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="F8" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>124</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>68</v>
@@ -2819,7 +2734,7 @@
         <v>71</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N8" s="9" t="s">
         <v>73</v>
@@ -2873,7 +2788,7 @@
         <v>85</v>
       </c>
       <c r="AE8" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AF8" s="10" t="s">
         <v>87</v>
@@ -2882,7 +2797,7 @@
         <v>70</v>
       </c>
       <c r="AH8" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AI8" s="10" t="s">
         <v>80</v>
@@ -2969,24 +2884,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:62 16357:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>100</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>68</v>
@@ -3007,7 +2922,7 @@
         <v>71</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N9" s="9" t="s">
         <v>73</v>
@@ -3055,10 +2970,10 @@
         <v>83</v>
       </c>
       <c r="AC9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD9" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="AD9" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="AE9" s="12" t="s">
         <v>86</v>
@@ -3070,7 +2985,7 @@
         <v>70</v>
       </c>
       <c r="AH9" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AI9" s="10" t="s">
         <v>80</v>
@@ -3157,48 +3072,48 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:62 16357:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="I10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="N10" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="O10" s="10" t="s">
         <v>74</v>
@@ -3345,48 +3260,48 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:62 16357:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="N11" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="O11" s="10" t="s">
         <v>74</v>
@@ -3431,10 +3346,10 @@
         <v>83</v>
       </c>
       <c r="AC11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD11" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="AD11" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="AE11" s="12" t="s">
         <v>86</v>
@@ -3534,12 +3449,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exception validation and Log added
</commit_message>
<xml_diff>
--- a/src/main/Configuration/Rules_V2.xlsx
+++ b/src/main/Configuration/Rules_V2.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M2_Sorbonne\Projet_Moteur\Rule_Engine\src\main\Configuration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,208 +26,208 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="125">
   <si>
-    <t xml:space="preserve">Workflow name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TYPE_TITRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TYPE_TITRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DATE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DATE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_STATUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_STATUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_SEXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_SEXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM_USUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM_USUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TAILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TAILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_VILLE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_VILLE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PAYS_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PAYS_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DEPARTEMENT_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DEPARTEMENT_NAISSSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_YEUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_YEUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_ORIGINE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_ORIGINE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_REPRESENTANT_LEGAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_REPRESANTANT_LEGAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_ADRESSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_ADRESSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_CODE_POSTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_CODE_POSTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_COMMUNE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_COMMUNE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TEL_PORTABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TEL_PORTABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DATE_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DATE_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_LIEU_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_LIEU_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NATIONALITE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NATIONALITE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DATE_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DATE_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_LIEU_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_LIEU_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NATIONALITE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NATIONALITE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande passeport mineur</t>
+    <t>Workflow name</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>REGLE_TYPE_TITRE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TYPE_TITRE</t>
+  </si>
+  <si>
+    <t>REGLE_DATE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DATE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM</t>
+  </si>
+  <si>
+    <t>REGLE_NOM</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM</t>
+  </si>
+  <si>
+    <t>REGLE_STATUT</t>
+  </si>
+  <si>
+    <t>MESSAGE_STATUT</t>
+  </si>
+  <si>
+    <t>REGLE_SEXE</t>
+  </si>
+  <si>
+    <t>MESSAGE_SEXE</t>
+  </si>
+  <si>
+    <t>REGLE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM_USUEL</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM_USUEL</t>
+  </si>
+  <si>
+    <t>REGLE_TAILLE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TAILLE</t>
+  </si>
+  <si>
+    <t>REGLE_VILLE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_VILLE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_PAYS_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_PAYS_NAISSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_DEPARTEMENT_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DEPARTEMENT_NAISSSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_YEUX</t>
+  </si>
+  <si>
+    <t>MESSAGE_YEUX</t>
+  </si>
+  <si>
+    <t>REGLE_ORIGINE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>MESSAGE_ORIGINE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>REGLE_REPRESENTANT_LEGAL</t>
+  </si>
+  <si>
+    <t>MESSAGE_REPRESANTANT_LEGAL</t>
+  </si>
+  <si>
+    <t>REGLE_ADRESSE</t>
+  </si>
+  <si>
+    <t>MESSAGE_ADRESSE</t>
+  </si>
+  <si>
+    <t>REGLE_CODE_POSTAL</t>
+  </si>
+  <si>
+    <t>MESSAGE_CODE_POSTAL</t>
+  </si>
+  <si>
+    <t>REGLE_COMMUNE</t>
+  </si>
+  <si>
+    <t>MESSAGE_COMMUNE</t>
+  </si>
+  <si>
+    <t>REGLE_TEL_PORTABLE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TEL_PORTABLE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_NOM_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_DATE_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DATE_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_LIEU_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_LIEU_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_NATIONALITE_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NATIONALITE_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_NOM_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_DATE_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DATE_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_LIEU_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_LIEU_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_NATIONALITE_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NATIONALITE_MERE</t>
+  </si>
+  <si>
+    <t>Première Demande passeport mineur</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP")</t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; Equal(value,"PSP")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. C’est une demande de passeport. Il doit contenir "PSP".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp;  Minor_Check(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Doit être un mineur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; Length_Between(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
+    <t>NotNull(value) &amp;&amp; Equal(value,"PSP")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. C’est une demande de passeport. Il doit contenir "PSP".</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp;  Minor_Check(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Doit être un mineur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; Length_Between(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
   </si>
   <si>
     <r>
@@ -244,7 +248,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">"</t>
+      <t>"</t>
     </r>
     <r>
       <rPr>
@@ -254,7 +258,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">mineur,MINEUR,Mineur</t>
+      <t>mineur,MINEUR,Mineur</t>
     </r>
     <r>
       <rPr>
@@ -264,7 +268,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">"</t>
+      <t>"</t>
     </r>
     <r>
       <rPr>
@@ -274,48 +278,48 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">)</t>
+      <t>)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ce champ est obligatoire et correspond l’un des mots suivant : mineur,MINEUR,Mineur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; BelongTo(value,"F,H,femme,homme,Femme,Homme,FEMME,HOMME")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et correspond l’un des mots suivant : F,H,femme,homme,Femme,Homme,FEMME,HOMME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(NotNull(value) &amp;&amp; Length_Between(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")) || IsNull(value)</t>
+    <t>Ce champ est obligatoire et correspond l’un des mots suivant : mineur,MINEUR,Mineur</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; BelongTo(value,"F,H,femme,homme,Femme,Homme,FEMME,HOMME")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et correspond l’un des mots suivant : F,H,femme,homme,Femme,Homme,FEMME,HOMME</t>
+  </si>
+  <si>
+    <t>(NotNull(value) &amp;&amp; Length_Between(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")) || IsNull(value)</t>
   </si>
   <si>
     <t xml:space="preserve"> La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; IsFloat(TAILLE)
+    <t>NotNull(value) &amp;&amp; IsFloat(TAILLE)
 &amp;&amp; Float_Between(value,0.5,3.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ce champ est obligatoire. La taille doit être dans un intervalle de 0,5 et 3,0m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( BornInFrance(PAYS_NAISSANCE) &amp;&amp; NotNull(value)   &amp;&amp; Length_Less_Than(value,3) &amp;&amp; IsNumber(value)) ||( !BornInFrance(PAYS_NAISSANCE) &amp;&amp; IsNull(value) )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si le champ PAYS_NAISSANCE est égale à France alors ce champ est obligatoire. La taille ne doit pas dépasser 3.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; BelongTo(value,"marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire et doit correspondre à l’un des valeur suivants : marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT</t>
+    <t>Ce champ est obligatoire. La taille doit être dans un intervalle de 0,5 et 3,0m</t>
+  </si>
+  <si>
+    <t>NotNull(value)</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire.</t>
+  </si>
+  <si>
+    <t>( BornInFrance(PAYS_NAISSANCE) &amp;&amp; NotNull(value)   &amp;&amp; Length_Less_Than(value,3) &amp;&amp; IsNumber(value)) ||( !BornInFrance(PAYS_NAISSANCE) &amp;&amp; IsNull(value) )</t>
+  </si>
+  <si>
+    <t>Si le champ PAYS_NAISSANCE est égale à France alors ce champ est obligatoire. La taille ne doit pas dépasser 3.</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; BelongTo(value,"marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT")</t>
+  </si>
+  <si>
+    <t>Le champ est obligatoire et doit correspondre à l’un des valeur suivants : marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT</t>
   </si>
   <si>
     <r>
@@ -336,95 +340,95 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
+      <t>NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Si le champ NOM_USAGE n’est pas vide alors ce champ est obligatoire et doit correspondre l’une des valeur suivants : Père,Mère,Époux,Épouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les carectère : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; IsNumber(value)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; IsNumber(value) &amp;&amp; LengthEqual(value,10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et doit être un nombre de 10 chiffres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
+    <t>Si le champ NOM_USAGE n’est pas vide alors ce champ est obligatoire et doit correspondre l’une des valeur suivants : Père,Mère,Époux,Épouse</t>
+  </si>
+  <si>
+    <t>Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les carectère : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; IsNumber(value)</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; IsNumber(value) &amp;&amp; LengthEqual(value,10)</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et doit être un nombre de 10 chiffres</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
   </si>
   <si>
     <t xml:space="preserve">NotNull(value) </t>
   </si>
   <si>
-    <t xml:space="preserve">Première Demande CNIE mineur</t>
+    <t>Première Demande CNIE mineur</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; Equal(value,"CNIE")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. C’est une demande de pièce d’identité. Il doit contenir "CNIE".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)&amp;&amp; BelongTo(value, "mineur,MINEUR,Mineur")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est toujours valide pour ce workflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande passeport adulte</t>
+    <t>NotNull(value) &amp;&amp; Equal(value,"CNIE")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. C’est une demande de pièce d’identité. Il doit contenir "CNIE".</t>
+  </si>
+  <si>
+    <t>NotNull(value)&amp;&amp; BelongTo(value, "mineur,MINEUR,Mineur")</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>Ce champ est toujours valide pour ce workflow</t>
+  </si>
+  <si>
+    <t>Première Demande passeport adulte</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" ) &amp;&amp;  Equal(TYPE_TITRE, "PSP")</t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; Major_Check(value)  &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Doit être un majeur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)&amp;&amp; BelongTo(value,"majeur,MAJEUR,Majeur")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et correspond l’un des mots suivant : majeur,MAJEUR,Majeur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande CNIE adulte</t>
+    <t>NotNull(value) &amp;&amp; Major_Check(value)  &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Doit être un majeur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>NotNull(value)&amp;&amp; BelongTo(value,"majeur,MAJEUR,Majeur")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et correspond l’un des mots suivant : majeur,MAJEUR,Majeur</t>
+  </si>
+  <si>
+    <t>Première Demande CNIE adulte</t>
   </si>
   <si>
     <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" )  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
   </si>
   <si>
-    <t xml:space="preserve">Première Demande passeport mineur emancipé</t>
+    <t>Première Demande passeport mineur emancipé</t>
   </si>
   <si>
     <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value)   &amp;&amp;  Minor_Check(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande CNIE mineur emancipé</t>
+    <t>NotNull(value)   &amp;&amp;  Minor_Check(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Première Demande CNIE mineur emancipé</t>
   </si>
   <si>
     <r>
@@ -459,13 +463,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Renouvellement passeport mineur</t>
+    <t>Renouvellement passeport mineur</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT, "mineur,MINEUR,Mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
   </si>
   <si>
-    <t xml:space="preserve">Ce champ est obligatoire. C’est une demande de passeport.Il doit contenir "PSP".</t>
+    <t>Ce champ est obligatoire. C’est une demande de passeport.Il doit contenir "PSP".</t>
   </si>
   <si>
     <t xml:space="preserve"> (NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
@@ -474,7 +478,7 @@
     <t xml:space="preserve">Le champ est obligatoire et la longueur doit être entre 1 et 76 </t>
   </si>
   <si>
-    <t xml:space="preserve">Renouvellement CNIE mineur</t>
+    <t>Renouvellement CNIE mineur</t>
   </si>
   <si>
     <r>
@@ -509,29 +513,26 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Renouvellement passeport adulte</t>
+    <t>Renouvellement passeport adulte</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" ) &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
   </si>
   <si>
-    <t xml:space="preserve">Renouvellement CNIE adulte</t>
+    <t>Renouvellement CNIE adulte</t>
   </si>
   <si>
     <t xml:space="preserve">  NotNull(DATE_NAISSANCE) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongTo(STATUT,"majeur,Majeur,MAJEUR" )  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
   </si>
   <si>
-    <t xml:space="preserve">Ce  champ est obligatoire. C’est une demande de pièce d’identité. Il doit contenir "CNIE".</t>
+    <t>Ce  champ est obligatoire. C’est une demande de pièce d’identité. Il doit contenir "CNIE".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,22 +541,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -604,15 +590,17 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="thin">
         <color rgb="FF5B9BD5"/>
@@ -622,7 +610,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -633,112 +621,78 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF5B9BD5"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF5B9BD5"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -797,60 +751,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -882,7 +852,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -906,7 +876,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -966,68 +936,66 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="64.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="27.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="61.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="66.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="48.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="62.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="21" style="2" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="90"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="90"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="2" width="40.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="74.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="33" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="41" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="45" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="51" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="55" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16351" min="63" style="2" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16354" min="16352" style="2" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16382" min="16355" style="0" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
+    <col min="1" max="1" width="44.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="61.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="54" style="2" customWidth="1"/>
+    <col min="9" max="9" width="66.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="54" style="2" customWidth="1"/>
+    <col min="11" max="11" width="63" style="2" customWidth="1"/>
+    <col min="12" max="12" width="31.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="72" style="2" customWidth="1"/>
+    <col min="14" max="14" width="31.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="48.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="54" style="2" customWidth="1"/>
+    <col min="17" max="17" width="62.21875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="54" style="2" customWidth="1"/>
+    <col min="19" max="20" width="31.44140625" style="2" customWidth="1"/>
+    <col min="21" max="23" width="22.44140625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="31.44140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="90" style="2" customWidth="1"/>
+    <col min="26" max="26" width="31.44140625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="81" style="2" customWidth="1"/>
+    <col min="28" max="28" width="31.44140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="90" style="2" customWidth="1"/>
+    <col min="30" max="30" width="40.44140625" style="2" customWidth="1"/>
+    <col min="31" max="31" width="74.44140625" style="2" customWidth="1"/>
+    <col min="32" max="32" width="54" style="2" customWidth="1"/>
+    <col min="33" max="40" width="31.44140625" style="2" customWidth="1"/>
+    <col min="41" max="44" width="54" style="2" customWidth="1"/>
+    <col min="45" max="50" width="31.44140625" style="2" customWidth="1"/>
+    <col min="51" max="54" width="54" style="2" customWidth="1"/>
+    <col min="55" max="62" width="31.44140625" style="2" customWidth="1"/>
+    <col min="63" max="16351" width="8.5546875" style="2"/>
+    <col min="16352" max="16354" width="10.109375" style="2" customWidth="1"/>
+    <col min="16355" max="16384" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:60 16355:16384" s="5" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1208,38 +1176,38 @@
       <c r="BH1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="XEA1" s="0"/>
-      <c r="XEB1" s="0"/>
-      <c r="XEC1" s="0"/>
-      <c r="XED1" s="0"/>
-      <c r="XEE1" s="0"/>
-      <c r="XEF1" s="0"/>
-      <c r="XEG1" s="0"/>
-      <c r="XEH1" s="0"/>
-      <c r="XEI1" s="0"/>
-      <c r="XEJ1" s="0"/>
-      <c r="XEK1" s="0"/>
-      <c r="XEL1" s="0"/>
-      <c r="XEM1" s="0"/>
-      <c r="XEN1" s="0"/>
-      <c r="XEO1" s="0"/>
-      <c r="XEP1" s="0"/>
-      <c r="XEQ1" s="0"/>
-      <c r="XER1" s="0"/>
-      <c r="XES1" s="0"/>
-      <c r="XET1" s="0"/>
-      <c r="XEU1" s="0"/>
-      <c r="XEV1" s="0"/>
-      <c r="XEW1" s="0"/>
-      <c r="XEX1" s="0"/>
-      <c r="XEY1" s="0"/>
-      <c r="XEZ1" s="0"/>
-      <c r="XFA1" s="0"/>
-      <c r="XFB1" s="0"/>
-      <c r="XFC1" s="0"/>
-      <c r="XFD1" s="0"/>
+      <c r="XEA1"/>
+      <c r="XEB1"/>
+      <c r="XEC1"/>
+      <c r="XED1"/>
+      <c r="XEE1"/>
+      <c r="XEF1"/>
+      <c r="XEG1"/>
+      <c r="XEH1"/>
+      <c r="XEI1"/>
+      <c r="XEJ1"/>
+      <c r="XEK1"/>
+      <c r="XEL1"/>
+      <c r="XEM1"/>
+      <c r="XEN1"/>
+      <c r="XEO1"/>
+      <c r="XEP1"/>
+      <c r="XEQ1"/>
+      <c r="XER1"/>
+      <c r="XES1"/>
+      <c r="XET1"/>
+      <c r="XEU1"/>
+      <c r="XEV1"/>
+      <c r="XEW1"/>
+      <c r="XEX1"/>
+      <c r="XEY1"/>
+      <c r="XEZ1"/>
+      <c r="XFA1"/>
+      <c r="XFB1"/>
+      <c r="XFC1"/>
+      <c r="XFD1"/>
     </row>
-    <row r="2" customFormat="false" ht="77.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:60 16355:16384" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1421,7 +1389,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:60 16355:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>93</v>
       </c>
@@ -1603,7 +1571,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:60 16355:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>100</v>
       </c>
@@ -1785,7 +1753,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:60 16355:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>106</v>
       </c>
@@ -1967,7 +1935,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:60 16355:16384" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>108</v>
       </c>
@@ -2149,7 +2117,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:60 16355:16384" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>111</v>
       </c>
@@ -2331,7 +2299,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:60 16355:16384" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>113</v>
       </c>
@@ -2513,7 +2481,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:60 16355:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>118</v>
       </c>
@@ -2695,7 +2663,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:60 16355:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>120</v>
       </c>
@@ -2877,7 +2845,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:60 16355:16384" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>122</v>
       </c>
@@ -3060,12 +3028,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
functions  &  log file added
</commit_message>
<xml_diff>
--- a/src/main/Configuration/Rules_V2.xlsx
+++ b/src/main/Configuration/Rules_V2.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M2_Sorbonne\Projet_Moteur\Rule_Engine\src\main\Configuration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,223 +26,223 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="125">
   <si>
-    <t xml:space="preserve">Workflow name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TYPE_TITRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TYPE_TITRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DATE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DATE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_STATUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_STATUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_SEXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_SEXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM_USUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM_USUEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TAILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TAILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_VILLE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_VILLE_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PAYS_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PAYS_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DEPARTEMENT_NAISSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DEPARTEMENT_NAISSSANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_YEUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_YEUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_ORIGINE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_ORIGINE_NOM_USAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_REPRESENTANT_LEGAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_REPRESANTANT_LEGAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_ADRESSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_ADRESSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_CODE_POSTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_CODE_POSTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_COMMUNE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_COMMUNE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_TEL_PORTABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_TEL_PORTABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DATE_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DATE_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_LIEU_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_LIEU_NAISSANCE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NATIONALITE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NATIONALITE_PERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_PRENOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_PRENOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NOM_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_DATE_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_DATE_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_LIEU_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_LIEU_NAISSANCE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGLE_NATIONALITE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESSAGE_NATIONALITE_MERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande passeport mineur</t>
+    <t>Workflow name</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>REGLE_TYPE_TITRE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TYPE_TITRE</t>
+  </si>
+  <si>
+    <t>REGLE_DATE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DATE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM</t>
+  </si>
+  <si>
+    <t>REGLE_NOM</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM</t>
+  </si>
+  <si>
+    <t>REGLE_STATUT</t>
+  </si>
+  <si>
+    <t>MESSAGE_STATUT</t>
+  </si>
+  <si>
+    <t>REGLE_SEXE</t>
+  </si>
+  <si>
+    <t>MESSAGE_SEXE</t>
+  </si>
+  <si>
+    <t>REGLE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM_USUEL</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM_USUEL</t>
+  </si>
+  <si>
+    <t>REGLE_TAILLE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TAILLE</t>
+  </si>
+  <si>
+    <t>REGLE_VILLE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_VILLE_NAISSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_PAYS_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_PAYS_NAISSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_DEPARTEMENT_NAISSANCE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DEPARTEMENT_NAISSSANCE</t>
+  </si>
+  <si>
+    <t>REGLE_YEUX</t>
+  </si>
+  <si>
+    <t>MESSAGE_YEUX</t>
+  </si>
+  <si>
+    <t>REGLE_ORIGINE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>MESSAGE_ORIGINE_NOM_USAGE</t>
+  </si>
+  <si>
+    <t>REGLE_REPRESENTANT_LEGAL</t>
+  </si>
+  <si>
+    <t>MESSAGE_REPRESANTANT_LEGAL</t>
+  </si>
+  <si>
+    <t>REGLE_ADRESSE</t>
+  </si>
+  <si>
+    <t>MESSAGE_ADRESSE</t>
+  </si>
+  <si>
+    <t>REGLE_CODE_POSTAL</t>
+  </si>
+  <si>
+    <t>MESSAGE_CODE_POSTAL</t>
+  </si>
+  <si>
+    <t>REGLE_COMMUNE</t>
+  </si>
+  <si>
+    <t>MESSAGE_COMMUNE</t>
+  </si>
+  <si>
+    <t>REGLE_TEL_PORTABLE</t>
+  </si>
+  <si>
+    <t>MESSAGE_TEL_PORTABLE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_NOM_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_DATE_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DATE_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_LIEU_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_LIEU_NAISSANCE_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_NATIONALITE_PERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NATIONALITE_PERE</t>
+  </si>
+  <si>
+    <t>REGLE_PRENOM_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_PRENOM_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_NOM_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NOM_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_DATE_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_DATE_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_LIEU_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_LIEU_NAISSANCE_MERE</t>
+  </si>
+  <si>
+    <t>REGLE_NATIONALITE_MERE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NATIONALITE_MERE</t>
+  </si>
+  <si>
+    <t>Première Demande passeport mineur</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT, "mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP")</t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; Equal(value,"PSP")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. C’est une demande de passeport. Il doit contenir "PSP".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp;  MinorCheck(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Doit être un mineur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; LengthBetween(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)&amp;&amp; BelongToCaseInsensitive(value, "mineur")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et correspond l’un des mots suivant : mineur,MINEUR,Mineur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; BelongTo(value,"F,H,femme,homme,Femme,Homme,FEMME,HOMME")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et correspond l’un des mots suivant : F,H,femme,homme,Femme,Homme,FEMME,HOMME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(NotNull(value) &amp;&amp; LengthBetween(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")) || IsNull(value)</t>
+    <t>NotNull(value) &amp;&amp; Equal(value,"PSP")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. C’est une demande de passeport. Il doit contenir "PSP".</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp;  MinorCheck(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Doit être un mineur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; LengthBetween(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
+  </si>
+  <si>
+    <t>NotNull(value)&amp;&amp; BelongToCaseInsensitive(value, "mineur")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et correspond l’un des mots suivant : mineur,MINEUR,Mineur</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; BelongTo(value,"F,H,femme,homme,Femme,Homme,FEMME,HOMME")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et correspond l’un des mots suivant : F,H,femme,homme,Femme,Homme,FEMME,HOMME</t>
+  </si>
+  <si>
+    <t>(NotNull(value) &amp;&amp; LengthBetween(value,1,76) &amp;&amp; ContainsOnlyCharacters(value,"ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ")) || IsNull(value)</t>
   </si>
   <si>
     <t xml:space="preserve"> La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
@@ -262,7 +266,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">FloatBetween</t>
+      <t>FloatBetween</t>
     </r>
     <r>
       <rPr>
@@ -272,29 +276,29 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(value,0.5,3.0)</t>
+      <t>(value,0.5,3.0)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ce champ est obligatoire. La taille doit être dans un intervalle de 0,5 et 3,0m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( BornInFrance(PAYS_NAISSANCE) &amp;&amp; NotNull(value)   &amp;&amp; LengthLessThan(value,3) &amp;&amp; IsNumber(value)) ||( !BornInFrance(PAYS_NAISSANCE) &amp;&amp; IsNull(value) )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si le champ PAYS_NAISSANCE est égale à France alors ce champ est obligatoire. La taille ne doit pas dépasser 3.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; BelongTo(value,"marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire et doit correspondre à l’un des valeur suivants : marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT</t>
+    <t>Ce champ est obligatoire. La taille doit être dans un intervalle de 0,5 et 3,0m</t>
+  </si>
+  <si>
+    <t>NotNull(value)</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire.</t>
+  </si>
+  <si>
+    <t>( BornInFrance(PAYS_NAISSANCE) &amp;&amp; NotNull(value)   &amp;&amp; LengthLessThan(value,3) &amp;&amp; IsNumber(value)) ||( !BornInFrance(PAYS_NAISSANCE) &amp;&amp; IsNull(value) )</t>
+  </si>
+  <si>
+    <t>Si le champ PAYS_NAISSANCE est égale à France alors ce champ est obligatoire. La taille ne doit pas dépasser 3.</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; BelongTo(value,"marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT")</t>
+  </si>
+  <si>
+    <t>Le champ est obligatoire et doit correspondre à l’un des valeur suivants : marron,Marron,MARRON,noir,Noir,NOIR,bleu,Bleu,BLEU,vert,Vert,VERT</t>
   </si>
   <si>
     <r>
@@ -315,108 +319,108 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
+      <t>NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Si le champ NOM_USAGE n’est pas vide alors ce champ est obligatoire et doit correspondre l’une des valeur suivants : Père,Mère,Époux,Épouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les carectère : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; IsNumber(value)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; IsNumber(value) &amp;&amp; LengthEqual(value,10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et doit être un nombre de 10 chiffres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
+    <t>Si le champ NOM_USAGE n’est pas vide alors ce champ est obligatoire et doit correspondre l’une des valeur suivants : Père,Mère,Époux,Épouse</t>
+  </si>
+  <si>
+    <t>Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les carectère : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; IsNumber(value)</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; IsNumber(value) &amp;&amp; LengthEqual(value,10)</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et doit être un nombre de 10 chiffres</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>Le champ est obligatoire. La longueur doit être entre 1 et 76 et doit contenir seulement les caractères : ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz»«\"'()-/.,ÀÁÂÃÄÅÆÇÈÉÊËÌÍÎÏÑÒÓÔÕÖÙÚÛÜÝŸŒàáâãäåæçèéêëìíîïñòóôõöùúûüýÿœ</t>
   </si>
   <si>
     <t xml:space="preserve">NotNull(value) </t>
   </si>
   <si>
-    <t xml:space="preserve">Première Demande CNIE mineur</t>
+    <t>Première Demande CNIE mineur</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT, "mineur") &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; Equal(value,"CNIE")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. C’est une demande de pièce d’identité. Il doit contenir "CNIE".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; IsFloat(TAILLE)
+    <t>NotNull(value) &amp;&amp; Equal(value,"CNIE")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. C’est une demande de pièce d’identité. Il doit contenir "CNIE".</t>
+  </si>
+  <si>
+    <t>NotNull(value) &amp;&amp; IsFloat(TAILLE)
 &amp;&amp; FloatBetween(value,0.5,3.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est toujours valide pour ce workflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande passeport adulte</t>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>Ce champ est toujours valide pour ce workflow</t>
+  </si>
+  <si>
+    <t>Première Demande passeport adulte</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT,"majeur" ) &amp;&amp;  Equal(TYPE_TITRE, "PSP")</t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; MajorCheck(value)  &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire. Doit être un majeur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value)&amp;&amp; BelongToCaseInsensitive(value,"majeur")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce champ est obligatoire et correspond l’un des mots suivant : majeur,MAJEUR,Majeur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande CNIE adulte</t>
+    <t>NotNull(value) &amp;&amp; MajorCheck(value)  &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire. Doit être un majeur. Le format valide : yyyy-MM-dd,dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>NotNull(value)&amp;&amp; BelongToCaseInsensitive(value,"majeur")</t>
+  </si>
+  <si>
+    <t>Ce champ est obligatoire et correspond l’un des mots suivant : majeur,MAJEUR,Majeur</t>
+  </si>
+  <si>
+    <t>Première Demande CNIE adulte</t>
   </si>
   <si>
     <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT,"majeur" )  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
   </si>
   <si>
-    <t xml:space="preserve">Première Demande passeport mineur emancipé</t>
+    <t>Première Demande passeport mineur emancipé</t>
   </si>
   <si>
     <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT, "mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
   </si>
   <si>
-    <t xml:space="preserve">NotNull(value)   &amp;&amp;  MinorCheck(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Première Demande CNIE mineur emancipé</t>
+    <t>NotNull(value)   &amp;&amp;  MinorCheck(value) &amp;&amp; DateBelongFormat(value,"yyyy-MM-dd,dd/MM/yyyy")</t>
+  </si>
+  <si>
+    <t>Première Demande CNIE mineur emancipé</t>
   </si>
   <si>
     <t xml:space="preserve">  NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT, "mineur")  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
   </si>
   <si>
-    <t xml:space="preserve">Renouvellement passeport mineur</t>
+    <t>Renouvellement passeport mineur</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT, "mineur") &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
   </si>
   <si>
-    <t xml:space="preserve">Ce champ est obligatoire. C’est une demande de passeport.Il doit contenir "PSP".</t>
+    <t>Ce champ est obligatoire. C’est une demande de passeport.Il doit contenir "PSP".</t>
   </si>
   <si>
     <t xml:space="preserve"> (NotNull(NOM_USAGE) &amp;&amp; NotNull(value) &amp;&amp; BelongTo(value,"Père,Mère,Époux,Épouse")) || (IsNull(NOM_USAGE) &amp;&amp; IsNull(value))</t>
@@ -425,35 +429,32 @@
     <t xml:space="preserve">Le champ est obligatoire et la longueur doit être entre 1 et 76 </t>
   </si>
   <si>
-    <t xml:space="preserve">Renouvellement CNIE mineur</t>
+    <t>Renouvellement CNIE mineur</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT, "mineur")  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
   </si>
   <si>
-    <t xml:space="preserve">Renouvellement passeport adulte</t>
+    <t>Renouvellement passeport adulte</t>
   </si>
   <si>
     <t xml:space="preserve"> NotNull(STATUT) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT,"majeur" ) &amp;&amp;  Equal(TYPE_TITRE, "PSP") </t>
   </si>
   <si>
-    <t xml:space="preserve">Renouvellement CNIE adulte</t>
+    <t>Renouvellement CNIE adulte</t>
   </si>
   <si>
     <t xml:space="preserve">  NotNull(DATE_NAISSANCE) &amp;&amp; NotNull(TYPE_TITRE) &amp;&amp; BelongToCaseInsensitive(STATUT,"majeur" )  &amp;&amp;  Equal(TYPE_TITRE, "CNIE") </t>
   </si>
   <si>
-    <t xml:space="preserve">Ce  champ est obligatoire. C’est une demande de pièce d’identité. Il doit contenir "CNIE".</t>
+    <t>Ce  champ est obligatoire. C’est une demande de pièce d’identité. Il doit contenir "CNIE".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,22 +463,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -526,15 +512,17 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="thin">
         <color rgb="FF5B9BD5"/>
@@ -544,7 +532,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -555,108 +543,75 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF5B9BD5"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF5B9BD5"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -715,60 +670,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -800,7 +771,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -824,7 +795,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -884,67 +855,66 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:BH11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XDZ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="6" sqref="B2:B11 C1:X1 Y1:Z11 AA1:AB1 AC1:AD11 AE1:BH1 E2"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="63.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="27.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="61.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="66.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="48.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="62.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="21" style="2" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="90"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="90"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="2" width="40.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="74.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="33" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="41" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="45" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="51" style="2" width="54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="55" style="2" width="31.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16351" min="63" style="2" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16354" min="16352" style="2" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16355" style="0" width="10.11"/>
+    <col min="1" max="1" width="44.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="61.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="54" style="2" customWidth="1"/>
+    <col min="9" max="9" width="66.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="54" style="2" customWidth="1"/>
+    <col min="11" max="11" width="63" style="2" customWidth="1"/>
+    <col min="12" max="12" width="31.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="72" style="2" customWidth="1"/>
+    <col min="14" max="14" width="31.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="48.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="54" style="2" customWidth="1"/>
+    <col min="17" max="17" width="62.21875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="54" style="2" customWidth="1"/>
+    <col min="19" max="20" width="31.44140625" style="2" customWidth="1"/>
+    <col min="21" max="23" width="22.44140625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="31.44140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="90" style="2" customWidth="1"/>
+    <col min="26" max="26" width="31.44140625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="81" style="2" customWidth="1"/>
+    <col min="28" max="28" width="31.44140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="90" style="2" customWidth="1"/>
+    <col min="30" max="30" width="40.44140625" style="2" customWidth="1"/>
+    <col min="31" max="31" width="74.44140625" style="2" customWidth="1"/>
+    <col min="32" max="32" width="54" style="2" customWidth="1"/>
+    <col min="33" max="40" width="31.44140625" style="2" customWidth="1"/>
+    <col min="41" max="44" width="54" style="2" customWidth="1"/>
+    <col min="45" max="50" width="31.44140625" style="2" customWidth="1"/>
+    <col min="51" max="54" width="54" style="2" customWidth="1"/>
+    <col min="55" max="62" width="31.44140625" style="2" customWidth="1"/>
+    <col min="63" max="16351" width="8.5546875" style="2"/>
+    <col min="16352" max="16354" width="10.109375" style="2" customWidth="1"/>
+    <col min="16355" max="16384" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:60" s="5" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1096,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="77.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:60" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1308,7 +1278,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:60" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>93</v>
       </c>
@@ -1490,7 +1460,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:60" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>100</v>
       </c>
@@ -1672,7 +1642,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:60" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>106</v>
       </c>
@@ -1854,7 +1824,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:60" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>108</v>
       </c>
@@ -2036,7 +2006,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:60" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>111</v>
       </c>
@@ -2218,7 +2188,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:60" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>113</v>
       </c>
@@ -2400,7 +2370,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:60" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>118</v>
       </c>
@@ -2582,7 +2552,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:60" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>120</v>
       </c>
@@ -2764,7 +2734,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:60" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>122</v>
       </c>
@@ -2947,12 +2917,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>